<commit_message>
order file upload function and design update
</commit_message>
<xml_diff>
--- a/app/Ref/prodcut_code.xlsx
+++ b/app/Ref/prodcut_code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sionp\Work\Dev\nextjs\order-dash\app\Ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CC2347-0A04-4B9F-A762-6F5C8495D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C488D3CE-A3A3-4602-892B-F4273E89A602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{86F13F7E-47CC-4100-A6D1-056BAF343162}"/>
   </bookViews>
@@ -798,9 +798,6 @@
     <t>P03890</t>
   </si>
   <si>
-    <t>Set Qty</t>
-  </si>
-  <si>
     <t>T2-3RUW-4AP4</t>
   </si>
   <si>
@@ -1510,6 +1507,10 @@
   </si>
   <si>
     <t>sales_price</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>set_qty</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1961,837 +1962,7 @@
     <cellStyle name="표준 2" xfId="1" xr:uid="{C440BE78-FBBC-4A86-93D3-6AC07CD76333}"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="149">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="66">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3765,7 +2936,7 @@
   <dimension ref="A1:G247"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.9"/>
@@ -3782,25 +2953,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>458</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F1" s="44" t="s">
         <v>23</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3808,13 +2979,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E2" s="10">
         <v>6240</v>
@@ -3831,13 +3002,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E3" s="10">
         <v>12850</v>
@@ -3854,13 +3025,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E4" s="10">
         <v>5240</v>
@@ -3877,13 +3048,13 @@
         <v>18</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5" s="8">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="10">
         <v>7150</v>
@@ -3900,13 +3071,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C6" s="8">
         <v>2</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E6" s="10">
         <v>6900</v>
@@ -3923,13 +3094,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E7" s="10">
         <v>10450</v>
@@ -3946,13 +3117,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E8" s="10">
         <v>6900</v>
@@ -3969,13 +3140,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="8">
         <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E9" s="10">
         <v>11430</v>
@@ -3992,13 +3163,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="8">
         <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" s="10">
         <v>13850</v>
@@ -4015,13 +3186,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C11" s="8">
         <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" s="10">
         <v>7240</v>
@@ -4038,13 +3209,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E12" s="10">
         <v>9600</v>
@@ -4061,13 +3232,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" s="8">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E13" s="10">
         <v>9710</v>
@@ -4081,16 +3252,16 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E14" s="10">
         <v>12830</v>
@@ -4107,13 +3278,13 @@
         <v>0</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C15" s="8">
         <v>2</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E15" s="10">
         <v>6900</v>
@@ -4127,16 +3298,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E16" s="10">
         <v>12830</v>
@@ -4153,13 +3324,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E17" s="10">
         <v>5620</v>
@@ -4176,13 +3347,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E18" s="10">
         <v>15500</v>
@@ -4199,13 +3370,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E19" s="10">
         <v>4440</v>
@@ -4219,7 +3390,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>191</v>
@@ -4245,13 +3416,13 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" s="8">
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E21" s="10">
         <v>11570</v>
@@ -4268,13 +3439,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E22" s="10">
         <v>8900</v>
@@ -4288,16 +3459,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E23" s="10">
         <v>4500</v>
@@ -4311,16 +3482,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" s="8">
         <v>1</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E24" s="10" t="e">
         <v>#N/A</v>
@@ -4334,16 +3505,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C25" s="8">
         <v>3</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E25" s="10">
         <v>9550</v>
@@ -4357,16 +3528,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" s="8">
         <v>2</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" s="10">
         <v>9660</v>
@@ -4380,7 +3551,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>213</v>
@@ -4406,20 +3577,20 @@
         <v>30</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C28" s="8">
         <v>2</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="45">
         <v>1.2</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -4427,20 +3598,20 @@
         <v>33</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C29" s="8">
         <v>1</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="45">
         <v>0.6</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -4448,20 +3619,20 @@
         <v>44</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C30" s="8">
         <v>2</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="45">
         <v>0.3</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4469,62 +3640,62 @@
         <v>96</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31" s="8">
         <v>1</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="45">
         <v>0.5</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="45">
         <v>0.2</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C33" s="8">
+        <v>1</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>293</v>
-      </c>
-      <c r="C33" s="8">
-        <v>1</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>294</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="45">
         <v>0.2</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -4532,20 +3703,20 @@
         <v>37</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C34" s="8">
         <v>2</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="45">
         <v>0.3</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -4553,20 +3724,20 @@
         <v>32</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C35" s="8">
         <v>2</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="45">
         <v>0.7</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -4574,20 +3745,20 @@
         <v>28</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C36" s="8">
         <v>1</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="45">
         <v>0.4</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -4595,20 +3766,20 @@
         <v>25</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C37" s="8">
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="45">
         <v>0.6</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -4616,20 +3787,20 @@
         <v>35</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C38" s="8">
         <v>2</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="45">
         <v>1.2</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -4637,20 +3808,20 @@
         <v>45</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C39" s="8">
         <v>1</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="45">
         <v>0.4</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -4658,20 +3829,20 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C40" s="8">
         <v>2</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="45">
         <v>1.4</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -4679,20 +3850,20 @@
         <v>41</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C41" s="8">
         <v>12</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="45">
         <v>1.6</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -4700,41 +3871,41 @@
         <v>43</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C42" s="8">
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="45">
         <v>0.6</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>297</v>
-      </c>
-      <c r="C43" s="8">
-        <v>1</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="45">
         <v>0.2</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -4742,25 +3913,25 @@
         <v>29</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C44" s="8">
         <v>1</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="45">
         <v>0.4</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>176</v>
@@ -4776,7 +3947,7 @@
         <v>0.5</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -4784,20 +3955,20 @@
         <v>47</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C46" s="8">
         <v>2</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="45">
         <v>1.2</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -4805,20 +3976,20 @@
         <v>34</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C47" s="8">
         <v>2</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E47" s="10"/>
       <c r="F47" s="45">
         <v>0.7</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -4826,20 +3997,20 @@
         <v>40</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="45">
         <v>0.6</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -4860,7 +4031,7 @@
         <v>0.3</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -4868,20 +4039,20 @@
         <v>42</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C50" s="8">
         <v>3</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E50" s="10"/>
       <c r="F50" s="45">
         <v>0.3</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -4889,41 +4060,41 @@
         <v>38</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C51" s="8">
         <v>1</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E51" s="10"/>
       <c r="F51" s="45">
         <v>0.1</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C52" s="8">
         <v>3</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E52" s="10"/>
       <c r="F52" s="45">
         <v>0.3</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -4931,20 +4102,20 @@
         <v>26</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C53" s="8">
         <v>2</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="45">
         <v>1.2</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -4952,20 +4123,20 @@
         <v>27</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C54" s="8">
         <v>1</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="45">
         <v>0.4</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -4973,20 +4144,20 @@
         <v>31</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C55" s="8">
         <v>1</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="45">
         <v>0.7</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -4994,20 +4165,20 @@
         <v>48</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C56" s="8">
         <v>2</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="45">
         <v>1.2</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -5015,62 +4186,62 @@
         <v>46</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C57" s="8">
         <v>2</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="45">
         <v>0.7</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C58" s="8">
         <v>12</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="45">
         <v>1.6</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C59" s="8">
         <v>12</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="45">
         <v>1.6</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -5078,20 +4249,20 @@
         <v>50</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C60" s="8">
         <v>1</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="45">
         <v>0.6</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -5099,20 +4270,20 @@
         <v>56</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C61" s="8">
         <v>1</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E61" s="10"/>
       <c r="F61" s="45">
         <v>0.6</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -5120,41 +4291,41 @@
         <v>49</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C62" s="8">
         <v>1</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E62" s="10"/>
       <c r="F62" s="45">
         <v>0.4</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C63" s="8">
         <v>2</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="45">
         <v>1.2</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -5162,20 +4333,20 @@
         <v>54</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C64" s="8">
         <v>1</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="45">
         <v>0.4</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -5183,20 +4354,20 @@
         <v>52</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C65" s="8">
         <v>2</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="45">
         <v>0.7</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -5204,20 +4375,20 @@
         <v>57</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C66" s="8">
         <v>2</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="45">
         <v>1.2</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -5225,20 +4396,20 @@
         <v>55</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C67" s="8">
         <v>1</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="45">
         <v>1.1000000000000001</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5246,20 +4417,20 @@
         <v>59</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C68" s="8">
         <v>1</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="45">
         <v>0.6</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -5267,20 +4438,20 @@
         <v>53</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C69" s="8">
         <v>1</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="45">
         <v>1.1000000000000001</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -5288,20 +4459,20 @@
         <v>63</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C70" s="8">
         <v>1</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E70" s="10"/>
       <c r="F70" s="45">
         <v>0.7</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -5309,41 +4480,41 @@
         <v>51</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C71" s="8">
         <v>2</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E71" s="10"/>
       <c r="F71" s="45">
         <v>0.7</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C72" s="8">
         <v>1</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="45">
         <v>0.6</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5351,20 +4522,20 @@
         <v>62</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C73" s="8">
         <v>1</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E73" s="10"/>
       <c r="F73" s="45">
         <v>0.6</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -5385,7 +4556,7 @@
         <v>0.2</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5393,20 +4564,20 @@
         <v>58</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C75" s="8">
         <v>2</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E75" s="10"/>
       <c r="F75" s="45">
         <v>1.4</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -5414,20 +4585,20 @@
         <v>64</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C76" s="8">
         <v>2</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E76" s="10"/>
       <c r="F76" s="45">
         <v>0.6</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5435,20 +4606,20 @@
         <v>60</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C77" s="8">
         <v>3</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E77" s="10"/>
       <c r="F77" s="45">
         <v>0.5</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -5456,13 +4627,13 @@
         <v>65</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C78" s="14">
         <v>1</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E78" s="10">
         <v>4690</v>
@@ -5479,13 +4650,13 @@
         <v>66</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C79" s="14">
         <v>2</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E79" s="10">
         <v>11900</v>
@@ -5502,13 +4673,13 @@
         <v>67</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C80" s="14">
         <v>1</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E80" s="10">
         <v>4490</v>
@@ -5525,13 +4696,13 @@
         <v>68</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C81" s="14">
         <v>1</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E81" s="10">
         <v>5320</v>
@@ -5548,13 +4719,13 @@
         <v>69</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C82" s="17">
         <v>1</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E82" s="10">
         <v>4980</v>
@@ -5571,13 +4742,13 @@
         <v>70</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C83" s="17">
         <v>2</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E83" s="10">
         <v>8700</v>
@@ -5594,13 +4765,13 @@
         <v>71</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C84" s="17">
         <v>1</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E84" s="10">
         <v>7600</v>
@@ -5617,13 +4788,13 @@
         <v>72</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C85" s="17">
         <v>2</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E85" s="10">
         <v>14500</v>
@@ -5637,16 +4808,16 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C86" s="17">
         <v>2</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E86" s="10">
         <v>13850</v>
@@ -5660,13 +4831,13 @@
         <v>73</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C87" s="17">
         <v>1</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E87" s="10">
         <v>14900</v>
@@ -5683,13 +4854,13 @@
         <v>74</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C88" s="17">
         <v>1</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E88" s="10">
         <v>15700</v>
@@ -5725,13 +4896,13 @@
         <v>76</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C90" s="17">
         <v>1</v>
       </c>
       <c r="D90" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E90" s="10">
         <v>6600</v>
@@ -5767,13 +4938,13 @@
         <v>78</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C92" s="17">
         <v>1</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E92" s="10">
         <v>7800</v>
@@ -5790,13 +4961,13 @@
         <v>79</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C93" s="17">
         <v>1</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E93" s="10">
         <v>11650</v>
@@ -5813,13 +4984,13 @@
         <v>80</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C94" s="17">
         <v>2</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E94" s="10">
         <v>14900</v>
@@ -5855,13 +5026,13 @@
         <v>82</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C96" s="14">
         <v>3</v>
       </c>
       <c r="D96" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E96" s="10">
         <v>16600</v>
@@ -5878,13 +5049,13 @@
         <v>83</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C97" s="14">
         <v>2</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E97" s="10">
         <v>9900</v>
@@ -5901,13 +5072,13 @@
         <v>84</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C98" s="14">
         <v>3</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E98" s="10">
         <v>11350</v>
@@ -5930,7 +5101,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E99" s="10">
         <v>2600</v>
@@ -5947,13 +5118,13 @@
         <v>86</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C100" s="17">
         <v>3</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E100" s="10">
         <v>11300</v>
@@ -5970,7 +5141,7 @@
         <v>87</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C101" s="17">
         <v>3</v>
@@ -6031,13 +5202,13 @@
         <v>97</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C104" s="17">
         <v>1</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E104" s="10">
         <v>9100</v>
@@ -6054,11 +5225,11 @@
         <v>98</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C105" s="17"/>
       <c r="D105" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E105" s="10">
         <v>3950</v>
@@ -6072,10 +5243,10 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B106" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="C106" s="17">
         <v>1</v>
@@ -6092,16 +5263,16 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B107" s="23" t="s">
+        <v>308</v>
+      </c>
+      <c r="C107" s="17">
+        <v>1</v>
+      </c>
+      <c r="D107" s="13" t="s">
         <v>307</v>
-      </c>
-      <c r="B107" s="23" t="s">
-        <v>309</v>
-      </c>
-      <c r="C107" s="17">
-        <v>1</v>
-      </c>
-      <c r="D107" s="13" t="s">
-        <v>308</v>
       </c>
       <c r="E107" s="10">
         <v>16100</v>
@@ -6514,13 +5685,13 @@
         <v>127</v>
       </c>
       <c r="B127" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C127" s="24">
+        <v>1</v>
+      </c>
+      <c r="D127" s="9" t="s">
         <v>417</v>
-      </c>
-      <c r="C127" s="24">
-        <v>1</v>
-      </c>
-      <c r="D127" s="9" t="s">
-        <v>418</v>
       </c>
       <c r="E127" s="10"/>
       <c r="F127" s="10">
@@ -6611,7 +5782,7 @@
         <v>0.2</v>
       </c>
       <c r="G131" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -7270,7 +6441,7 @@
         <v>158</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C163" s="24">
         <v>1</v>
@@ -7480,13 +6651,13 @@
         <v>166</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C173" s="24">
         <v>6</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E173" s="10"/>
       <c r="F173" s="10">
@@ -7708,16 +6879,16 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B184" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="B184" s="7" t="s">
+      <c r="C184" s="25">
+        <v>1</v>
+      </c>
+      <c r="D184" s="9" t="s">
         <v>303</v>
-      </c>
-      <c r="C184" s="25">
-        <v>1</v>
-      </c>
-      <c r="D184" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="E184" s="10"/>
       <c r="F184" s="10">
@@ -7729,28 +6900,28 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C185" s="25">
+        <v>1</v>
+      </c>
+      <c r="D185" s="9" t="s">
         <v>312</v>
-      </c>
-      <c r="B185" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C185" s="25">
-        <v>1</v>
-      </c>
-      <c r="D185" s="9" t="s">
-        <v>313</v>
       </c>
       <c r="E185" s="11"/>
       <c r="F185" s="10">
         <v>0.3</v>
       </c>
       <c r="G185" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B186" s="7" t="s">
         <v>176</v>
@@ -7773,10 +6944,10 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B187" s="7" t="s">
         <v>322</v>
-      </c>
-      <c r="B187" s="7" t="s">
-        <v>323</v>
       </c>
       <c r="C187" s="25">
         <v>2</v>
@@ -7789,33 +6960,33 @@
         <v>0.7</v>
       </c>
       <c r="G187" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="188" spans="1:7">
       <c r="A188" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C188" s="25">
         <v>6</v>
       </c>
       <c r="D188" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E188" s="11"/>
       <c r="F188" s="10">
         <v>0.6</v>
       </c>
       <c r="G188" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="189" spans="1:7">
       <c r="A189" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B189" s="7" t="s">
         <v>221</v>
@@ -7838,16 +7009,16 @@
     </row>
     <row r="190" spans="1:7">
       <c r="A190" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B190" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="C190" s="25">
+        <v>1</v>
+      </c>
+      <c r="D190" s="21" t="s">
         <v>328</v>
-      </c>
-      <c r="B190" s="21" t="s">
-        <v>330</v>
-      </c>
-      <c r="C190" s="25">
-        <v>1</v>
-      </c>
-      <c r="D190" s="21" t="s">
-        <v>329</v>
       </c>
       <c r="E190" s="10">
         <v>2600</v>
@@ -7861,394 +7032,394 @@
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B191" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C191" s="25">
         <v>2</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E191" s="11"/>
       <c r="F191" s="45">
         <v>0.6</v>
       </c>
       <c r="G191" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B192" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C192" s="25">
         <v>1</v>
       </c>
       <c r="D192" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E192" s="11"/>
       <c r="F192" s="45">
         <v>0.3</v>
       </c>
       <c r="G192" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="193" spans="1:7">
       <c r="A193" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B193" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C193" s="25">
         <v>1</v>
       </c>
       <c r="D193" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E193" s="11"/>
       <c r="F193" s="45">
         <v>0.3</v>
       </c>
       <c r="G193" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="194" spans="1:7">
       <c r="A194" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B194" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C194" s="25">
         <v>1</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E194" s="11"/>
       <c r="F194" s="45">
         <v>0.3</v>
       </c>
       <c r="G194" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="195" spans="1:7">
       <c r="A195" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B195" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C195" s="25">
         <v>1</v>
       </c>
       <c r="D195" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E195" s="11"/>
       <c r="F195" s="45">
         <v>0.3</v>
       </c>
       <c r="G195" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="196" spans="1:7">
       <c r="A196" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B196" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C196" s="25">
         <v>1</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E196" s="11"/>
       <c r="F196" s="45">
         <v>0.7</v>
       </c>
       <c r="G196" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="197" spans="1:7">
       <c r="A197" s="21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B197" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C197" s="25">
         <v>1</v>
       </c>
       <c r="D197" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E197" s="11"/>
       <c r="F197" s="45">
         <v>0.7</v>
       </c>
       <c r="G197" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="198" spans="1:7">
       <c r="A198" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B198" s="31" t="s">
         <v>346</v>
       </c>
-      <c r="B198" s="31" t="s">
-        <v>347</v>
-      </c>
       <c r="C198" s="25">
         <v>1</v>
       </c>
       <c r="D198" s="29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E198" s="11"/>
       <c r="F198" s="45">
         <v>0.3</v>
       </c>
       <c r="G198" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="199" spans="1:7">
       <c r="A199" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B199" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C199" s="25">
         <v>2</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E199" s="11"/>
       <c r="F199" s="45">
         <v>0.6</v>
       </c>
       <c r="G199" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="200" spans="1:7">
       <c r="A200" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C200" s="34">
         <v>1</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E200" s="11"/>
       <c r="F200" s="46">
         <v>0.6</v>
       </c>
       <c r="G200" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="201" spans="1:7">
       <c r="A201" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="B201" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="B201" s="33" t="s">
-        <v>351</v>
-      </c>
       <c r="C201" s="34">
         <v>1</v>
       </c>
       <c r="D201" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E201" s="11"/>
       <c r="F201" s="46">
         <v>0.4</v>
       </c>
       <c r="G201" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="202" spans="1:7">
       <c r="A202" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="B202" s="35" t="s">
         <v>352</v>
       </c>
-      <c r="B202" s="35" t="s">
-        <v>353</v>
-      </c>
       <c r="C202" s="34">
         <v>1</v>
       </c>
       <c r="D202" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E202" s="11"/>
       <c r="F202" s="46">
         <v>0.8</v>
       </c>
       <c r="G202" s="35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="203" spans="1:7">
       <c r="A203" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B203" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="B203" s="29" t="s">
-        <v>355</v>
-      </c>
       <c r="C203" s="25">
         <v>1</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E203" s="11"/>
       <c r="F203" s="46">
         <v>0.4</v>
       </c>
       <c r="G203" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="204" spans="1:7">
       <c r="A204" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B204" s="29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C204" s="25">
         <v>4</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E204" s="11"/>
       <c r="F204" s="46">
         <v>0.5</v>
       </c>
       <c r="G204" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="205" spans="1:7">
       <c r="A205" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B205" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="B205" s="29" t="s">
-        <v>357</v>
-      </c>
       <c r="C205" s="25">
         <v>1</v>
       </c>
       <c r="D205" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E205" s="11"/>
       <c r="F205" s="46">
         <v>0.4</v>
       </c>
       <c r="G205" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="B206" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="B206" s="29" t="s">
-        <v>359</v>
-      </c>
       <c r="C206" s="25">
         <v>1</v>
       </c>
       <c r="D206" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E206" s="11"/>
       <c r="F206" s="46">
         <v>0.7</v>
       </c>
       <c r="G206" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C207" s="25">
         <v>3</v>
       </c>
       <c r="D207" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E207" s="11"/>
       <c r="F207" s="46">
         <v>0.5</v>
       </c>
       <c r="G207" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B208" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="B208" s="29" t="s">
-        <v>361</v>
-      </c>
       <c r="C208" s="25">
         <v>1</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E208" s="11"/>
       <c r="F208" s="46">
         <v>0.7</v>
       </c>
       <c r="G208" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="B209" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B209" s="6" t="s">
+      <c r="C209" s="25">
+        <v>1</v>
+      </c>
+      <c r="D209" s="26" t="s">
         <v>364</v>
-      </c>
-      <c r="C209" s="25">
-        <v>1</v>
-      </c>
-      <c r="D209" s="26" t="s">
-        <v>365</v>
       </c>
       <c r="E209" s="10">
         <v>9960</v>
@@ -8262,16 +7433,16 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C210" s="25">
         <v>4</v>
       </c>
       <c r="D210" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E210" s="10">
         <v>13420</v>
@@ -8285,91 +7456,91 @@
     </row>
     <row r="211" spans="1:7">
       <c r="A211" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B211" s="29" t="s">
         <v>366</v>
       </c>
-      <c r="B211" s="29" t="s">
-        <v>367</v>
-      </c>
       <c r="C211" s="25">
         <v>1</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E211" s="11"/>
       <c r="F211" s="45">
         <v>0.6</v>
       </c>
       <c r="G211" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="212" spans="1:7">
       <c r="A212" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B212" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C212" s="25">
         <v>1</v>
       </c>
       <c r="D212" s="12" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E212" s="11"/>
       <c r="F212" s="45">
         <v>0.6</v>
       </c>
       <c r="G212" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="213" spans="1:7">
       <c r="A213" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B213" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B213" s="7" t="s">
-        <v>372</v>
-      </c>
       <c r="C213" s="25">
         <v>1</v>
       </c>
       <c r="D213" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E213" s="11"/>
       <c r="F213" s="45">
         <v>0.4</v>
       </c>
       <c r="G213" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="214" spans="1:7">
       <c r="A214" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B214" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="B214" s="6" t="s">
+      <c r="C214" s="25">
+        <v>1</v>
+      </c>
+      <c r="D214" s="37" t="s">
         <v>374</v>
-      </c>
-      <c r="C214" s="25">
-        <v>1</v>
-      </c>
-      <c r="D214" s="37" t="s">
-        <v>375</v>
       </c>
       <c r="E214" s="11"/>
       <c r="F214" s="45">
         <v>0.2</v>
       </c>
       <c r="G214" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="215" spans="1:7">
       <c r="A215" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B215" s="7" t="s">
         <v>213</v>
@@ -8378,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="D215" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E215" s="10">
         <v>4060</v>
@@ -8392,16 +7563,16 @@
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C216" s="25">
         <v>1</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E216" s="10">
         <v>12850</v>
@@ -8410,21 +7581,21 @@
         <v>0.6</v>
       </c>
       <c r="G216" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B217" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="B217" s="29" t="s">
-        <v>382</v>
-      </c>
       <c r="C217" s="25">
         <v>1</v>
       </c>
       <c r="D217" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E217" s="38">
         <v>6900</v>
@@ -8433,21 +7604,21 @@
         <v>0.4</v>
       </c>
       <c r="G217" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B218" s="29" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C218" s="25">
         <v>1</v>
       </c>
       <c r="D218" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E218" s="6">
         <v>8390</v>
@@ -8456,21 +7627,21 @@
         <v>0.4</v>
       </c>
       <c r="G218" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="219" spans="1:7">
       <c r="A219" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>384</v>
-      </c>
-      <c r="B219" s="12" t="s">
-        <v>385</v>
       </c>
       <c r="C219" s="25">
         <v>2</v>
       </c>
       <c r="D219" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E219" s="6">
         <v>6990</v>
@@ -8479,21 +7650,21 @@
         <v>0.8</v>
       </c>
       <c r="G219" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="220" spans="1:7">
       <c r="A220" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C220" s="25">
         <v>2</v>
       </c>
       <c r="D220" s="26" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E220" s="6">
         <v>12850</v>
@@ -8507,16 +7678,16 @@
     </row>
     <row r="221" spans="1:7">
       <c r="A221" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C221" s="25">
         <v>3</v>
       </c>
       <c r="D221" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E221" s="10">
         <v>11350</v>
@@ -8530,37 +7701,37 @@
     </row>
     <row r="222" spans="1:7">
       <c r="A222" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B222" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C222" s="25">
         <v>3</v>
       </c>
       <c r="D222" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E222" s="11"/>
       <c r="F222" s="45">
         <v>0.6</v>
       </c>
       <c r="G222" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="223" spans="1:7">
       <c r="A223" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B223" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C223" s="25">
         <v>1</v>
       </c>
       <c r="D223" s="39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F223" s="45">
         <v>0.3</v>
@@ -8571,16 +7742,16 @@
     </row>
     <row r="224" spans="1:7" ht="16.3" thickBot="1">
       <c r="A224" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B224" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C224" s="25">
         <v>1</v>
       </c>
       <c r="D224" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F224" s="45">
         <v>0.3</v>
@@ -8591,16 +7762,16 @@
     </row>
     <row r="225" spans="1:7" ht="16.3" thickBot="1">
       <c r="A225" s="42" t="s">
+        <v>398</v>
+      </c>
+      <c r="B225" s="41" t="s">
         <v>399</v>
       </c>
-      <c r="B225" s="41" t="s">
-        <v>400</v>
-      </c>
       <c r="C225" s="25">
         <v>1</v>
       </c>
       <c r="D225" s="40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G225" s="15" t="s">
         <v>24</v>
@@ -8608,52 +7779,52 @@
     </row>
     <row r="226" spans="1:7" ht="18.45">
       <c r="A226" s="43" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C226" s="25">
         <v>1</v>
       </c>
       <c r="D226" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E226"/>
       <c r="G226" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="18.45">
       <c r="A227" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="B227" s="15" t="s">
         <v>402</v>
-      </c>
-      <c r="B227" s="15" t="s">
-        <v>403</v>
       </c>
       <c r="C227" s="25">
         <v>2</v>
       </c>
       <c r="D227" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E227"/>
       <c r="G227" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="18.45">
       <c r="A228" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C228" s="25">
         <v>2</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E228" s="10">
         <v>7150</v>
@@ -8667,56 +7838,56 @@
     </row>
     <row r="229" spans="1:7" ht="18.45">
       <c r="A229" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="B229" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="B229" s="48" t="s">
-        <v>409</v>
-      </c>
       <c r="C229" s="25">
         <v>1</v>
       </c>
       <c r="D229" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F229" s="45">
         <v>0.3</v>
       </c>
       <c r="G229" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="18.45">
       <c r="A230" t="s">
+        <v>409</v>
+      </c>
+      <c r="B230" t="s">
+        <v>411</v>
+      </c>
+      <c r="C230" s="25">
+        <v>1</v>
+      </c>
+      <c r="D230" s="26" t="s">
         <v>410</v>
-      </c>
-      <c r="B230" t="s">
-        <v>412</v>
-      </c>
-      <c r="C230" s="25">
-        <v>1</v>
-      </c>
-      <c r="D230" s="26" t="s">
-        <v>411</v>
       </c>
       <c r="F230" s="45">
         <v>0.2</v>
       </c>
       <c r="G230" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="18.899999999999999" thickBot="1">
       <c r="A231" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C231" s="25">
         <v>1</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F231" s="45">
         <v>0.2</v>
@@ -8727,30 +7898,30 @@
     </row>
     <row r="232" spans="1:7" ht="18.899999999999999" thickBot="1">
       <c r="A232" t="s">
+        <v>414</v>
+      </c>
+      <c r="B232" s="50" t="s">
+        <v>413</v>
+      </c>
+      <c r="C232" s="25">
+        <v>1</v>
+      </c>
+      <c r="D232" s="49" t="s">
         <v>415</v>
-      </c>
-      <c r="B232" s="50" t="s">
-        <v>414</v>
-      </c>
-      <c r="C232" s="25">
-        <v>1</v>
-      </c>
-      <c r="D232" s="49" t="s">
-        <v>416</v>
       </c>
       <c r="F232" s="45">
         <v>0.3</v>
       </c>
       <c r="G232" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="16.3" thickBot="1">
       <c r="A233" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="B233" s="50" t="s">
         <v>419</v>
-      </c>
-      <c r="B233" s="50" t="s">
-        <v>420</v>
       </c>
       <c r="C233" s="25">
         <v>1</v>
@@ -8767,16 +7938,16 @@
     </row>
     <row r="234" spans="1:7" ht="16.3" thickBot="1">
       <c r="A234" s="51" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B234" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C234" s="25">
         <v>1</v>
       </c>
       <c r="D234" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G234" s="15" t="s">
         <v>94</v>
@@ -8784,16 +7955,16 @@
     </row>
     <row r="235" spans="1:7" ht="16.3" thickBot="1">
       <c r="A235" s="51" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B235" s="52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C235" s="25">
         <v>1</v>
       </c>
       <c r="D235" s="52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G235" s="15" t="s">
         <v>94</v>
@@ -8801,7 +7972,7 @@
     </row>
     <row r="236" spans="1:7" ht="16.3" thickBot="1">
       <c r="A236" s="51" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B236" s="52" t="s">
         <v>188</v>
@@ -8818,10 +7989,10 @@
     </row>
     <row r="237" spans="1:7" ht="16.3" thickBot="1">
       <c r="A237" s="51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B237" s="52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C237" s="25">
         <v>1</v>
@@ -8835,16 +8006,16 @@
     </row>
     <row r="238" spans="1:7" ht="16.3" thickBot="1">
       <c r="A238" s="51" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B238" s="52" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C238" s="25">
         <v>1</v>
       </c>
       <c r="D238" s="52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G238" s="15" t="s">
         <v>94</v>
@@ -8852,16 +8023,16 @@
     </row>
     <row r="239" spans="1:7" ht="16.3" thickBot="1">
       <c r="A239" s="51" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B239" s="52" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C239" s="25">
         <v>1</v>
       </c>
       <c r="D239" s="52" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G239" s="15" t="s">
         <v>94</v>
@@ -8869,16 +8040,16 @@
     </row>
     <row r="240" spans="1:7" ht="16.3" thickBot="1">
       <c r="A240" s="51" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B240" s="52" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C240" s="25">
         <v>1</v>
       </c>
       <c r="D240" s="52" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G240" s="15" t="s">
         <v>94</v>
@@ -8886,16 +8057,16 @@
     </row>
     <row r="241" spans="1:7" ht="16.3" thickBot="1">
       <c r="A241" s="51" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B241" s="52" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C241" s="25">
         <v>4</v>
       </c>
       <c r="D241" s="52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G241" s="15" t="s">
         <v>94</v>
@@ -8903,16 +8074,16 @@
     </row>
     <row r="242" spans="1:7" ht="16.3" thickBot="1">
       <c r="A242" s="51" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B242" s="52" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C242" s="25">
         <v>1</v>
       </c>
       <c r="D242" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G242" s="15" t="s">
         <v>94</v>
@@ -8920,16 +8091,16 @@
     </row>
     <row r="243" spans="1:7" ht="16.3" thickBot="1">
       <c r="A243" s="51" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B243" s="52" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C243" s="25">
         <v>1</v>
       </c>
       <c r="D243" s="52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G243" s="15" t="s">
         <v>94</v>
@@ -8937,24 +8108,24 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244" s="54" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B244" s="53" t="s">
+        <v>443</v>
+      </c>
+      <c r="C244" s="25">
+        <v>1</v>
+      </c>
+      <c r="D244" s="54" t="s">
         <v>444</v>
       </c>
-      <c r="C244" s="25">
-        <v>1</v>
-      </c>
-      <c r="D244" s="54" t="s">
-        <v>445</v>
-      </c>
       <c r="G244" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B245" s="53" t="s">
         <v>106</v>
@@ -8968,33 +8139,33 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="B246" s="53" t="s">
+        <v>449</v>
+      </c>
+      <c r="C246" s="25">
+        <v>1</v>
+      </c>
+      <c r="D246" s="53" t="s">
+        <v>448</v>
+      </c>
+      <c r="G246" s="15" t="s">
         <v>451</v>
-      </c>
-      <c r="B246" s="53" t="s">
-        <v>450</v>
-      </c>
-      <c r="C246" s="25">
-        <v>1</v>
-      </c>
-      <c r="D246" s="53" t="s">
-        <v>449</v>
-      </c>
-      <c r="G246" s="15" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="247" spans="1:7">
       <c r="A247" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="B247" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="B247" s="6" t="s">
+      <c r="C247" s="25">
+        <v>1</v>
+      </c>
+      <c r="D247" s="26" t="s">
         <v>454</v>
-      </c>
-      <c r="C247" s="25">
-        <v>1</v>
-      </c>
-      <c r="D247" s="26" t="s">
-        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -9003,23 +8174,23 @@
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="65" priority="98"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A245:A1048576 A1:A243">
-    <cfRule type="duplicateValues" dxfId="64" priority="20"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78 A80:A88">
     <cfRule type="duplicateValues" dxfId="63" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:A107">
-    <cfRule type="duplicateValues" dxfId="62" priority="80"/>
-    <cfRule type="duplicateValues" dxfId="61" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206">
     <cfRule type="duplicateValues" dxfId="60" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A210">
     <cfRule type="duplicateValues" dxfId="59" priority="174"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="175"/>
-    <cfRule type="duplicateValues" dxfId="57" priority="176"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="176"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="175"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A1:A228 A230:A233">
     <cfRule type="duplicateValues" dxfId="56" priority="23"/>
@@ -9027,98 +8198,98 @@
   <conditionalFormatting sqref="A245:A1048576 A1:A233">
     <cfRule type="duplicateValues" dxfId="55" priority="21"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A245:A1048576 A1:A243">
+    <cfRule type="duplicateValues" dxfId="54" priority="20"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A1:A218 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="54" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A1:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="53" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="51" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A1:A215 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="50" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="49" priority="43"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="47" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A214:A215 A1:A200 A202:A205 A207:A208 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="46" priority="189"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="189"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A214:A215 A1:A205 A207:A208 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="45" priority="194"/>
     <cfRule type="duplicateValues" dxfId="44" priority="195"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="194"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A214:A215 A1:A208 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="43" priority="202"/>
     <cfRule type="duplicateValues" dxfId="42" priority="203"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="202"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A214:A215 A184:A200 A1 A202:A205 A207:A208 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="41" priority="208"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="208"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A245:A1048576 A226:A228 A217:A218 A214:A215 A184:A200 A1:A24 A28:A107 A202:A205 A207:A208 A220:A224 A230:A233">
-    <cfRule type="duplicateValues" dxfId="40" priority="214"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="214"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D191:D197">
-    <cfRule type="duplicateValues" dxfId="39" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D199">
-    <cfRule type="duplicateValues" dxfId="37" priority="74"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D200">
-    <cfRule type="duplicateValues" dxfId="35" priority="71"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="33" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D203:D204">
-    <cfRule type="duplicateValues" dxfId="32" priority="64"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="65"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="66"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="67"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D205">
-    <cfRule type="duplicateValues" dxfId="27" priority="59"/>
     <cfRule type="duplicateValues" dxfId="26" priority="60"/>
     <cfRule type="duplicateValues" dxfId="25" priority="61"/>
     <cfRule type="duplicateValues" dxfId="24" priority="62"/>
     <cfRule type="duplicateValues" dxfId="23" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D208">
-    <cfRule type="duplicateValues" dxfId="22" priority="50"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="54"/>
     <cfRule type="duplicateValues" dxfId="19" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="54"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D217:D218">
-    <cfRule type="duplicateValues" dxfId="16" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="32"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="40"/>
     <cfRule type="duplicateValues" dxfId="10" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="39"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D222">
-    <cfRule type="duplicateValues" dxfId="4" priority="27"/>
     <cfRule type="duplicateValues" dxfId="3" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D247:D1048576 D213 D209:D210 A216 D215:D216 D220:D222 D224 D226:D228 D230:D231 D1:D206">
-    <cfRule type="duplicateValues" dxfId="2" priority="215"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="215"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D247:D1048576 D230:D231 D1:D228">
-    <cfRule type="duplicateValues" dxfId="1" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>